<commit_message>
prochur update nijeo specifically janina
</commit_message>
<xml_diff>
--- a/BloodSampleMother/DB and Documents/MSCForm3.xlsx
+++ b/BloodSampleMother/DB and Documents/MSCForm3.xlsx
@@ -2548,7 +2548,7 @@
         <v>91</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="R19" s="16" t="s">
         <v>33</v>
@@ -2562,7 +2562,7 @@
       <c r="U19" s="16"/>
       <c r="V19" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('18', 'q17','frmsinglechoice', 'tblMainQues','','17. Plasma Sample Hemolyzed?(Plasma is red, not yellow)(Note: Only for maternal venous blood samples (type B))','','END','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('18', 'q17','frmsinglechoice', 'tblMainQues','','17. Plasma Sample Hemolyzed?(Plasma is red, not yellow)(Note: Only for maternal venous blood samples (type B))','','q18h1','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
       </c>
     </row>
     <row r="20" spans="1:22">

</xml_diff>